<commit_message>
add default bounds for FBA reaction fluxes
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37580" windowHeight="21140" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>For testing</t>
+  </si>
+  <si>
+    <t>Min flux</t>
+  </si>
+  <si>
+    <t>Max flux</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1361,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1833,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1848,7 +1854,7 @@
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -1864,14 +1870,20 @@
       <c r="E1" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1884,13 +1896,19 @@
       <c r="D2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1903,13 +1921,15 @@
       <c r="D3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1922,13 +1942,15 @@
       <c r="D4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1941,11 +1963,13 @@
       <c r="D5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D5">

</xml_diff>

<commit_message>
handle models with or without water full test coverage of class DynamicModel, SimulationObject
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-14420" yWindow="22060" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -440,6 +440,18 @@
   </si>
   <si>
     <t>Max flux</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>metabolite</t>
+  </si>
+  <si>
+    <t>H2O[e]</t>
+  </si>
+  <si>
+    <t>H2O[c]</t>
   </si>
 </sst>
 </file>
@@ -582,7 +594,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -627,6 +639,9 @@
     <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="12" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1536,10 +1551,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="147" zoomScaleNormal="147" zoomScalePageLayoutView="147" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1735,6 +1750,23 @@
         <v>76</v>
       </c>
     </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="19">
+        <v>18.0152</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J6">
     <sortState ref="A2:L147">
@@ -1749,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="184" zoomScaleNormal="184" zoomScalePageLayoutView="184" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" zoomScalePageLayoutView="184" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1828,6 +1860,22 @@
         <v>2E-3</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B5">
     <sortCondition ref="A2:A5"/>
@@ -1841,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating for new units attribute of wc_lang.Concentration
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,14 +34,19 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="144">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -259,9 +264,15 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_1[e]</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_2[e]</t>
   </si>
   <si>
@@ -280,6 +291,9 @@
     <t xml:space="preserve">H2O[e]</t>
   </si>
   <si>
+    <t xml:space="preserve">molecules</t>
+  </si>
+  <si>
     <t xml:space="preserve">H2O[c]</t>
   </si>
   <si>
@@ -413,9 +427,6 @@
   </si>
   <si>
     <t xml:space="preserve">Submodels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
   </si>
   <si>
     <t xml:space="preserve">fractionDryWeight</t>
@@ -772,7 +783,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -865,25 +876,25 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -894,24 +905,24 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>2000</v>
@@ -920,13 +931,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D4" s="5" t="n">
         <v>0.0003</v>
@@ -937,13 +948,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>0.0003</v>
@@ -954,13 +965,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="5" t="n">
         <v>0.0003</v>
@@ -993,13 +1004,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="13" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="13" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="13" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -1014,10 +1025,10 @@
         <v>23</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>13</v>
@@ -1028,10 +1039,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>29</v>
@@ -1043,16 +1054,16 @@
         <v>45</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>29</v>
@@ -1066,10 +1077,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>29</v>
@@ -1083,10 +1094,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>29</v>
@@ -1122,8 +1133,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="13" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -1149,13 +1160,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1182,12 +1193,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="42.7408906882591"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="48.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="2" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1202,13 +1213,13 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>13</v>
@@ -1219,10 +1230,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1231,10 +1242,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1288,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>13</v>
@@ -1308,9 +1319,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="2" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="2" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1325,46 +1336,46 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>13</v>
@@ -1401,10 +1412,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -1413,22 +1424,22 @@
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1527,13 +1538,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="8.78542510121457"/>
@@ -1636,9 +1647,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="2" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="44.4534412955466"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="2" width="8.78542510121457"/>
   </cols>
@@ -1724,12 +1735,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="2" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="14.7813765182186"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="2" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="2" width="18.6396761133603"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="2" width="8.78542510121457"/>
   </cols>
@@ -1950,21 +1961,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="184" zoomScaleNormal="184" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="184" zoomScaleNormal="184" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="2" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="2" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="2" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="2" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1975,74 +1986,101 @@
         <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>0.000148</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>0.0002</v>
       </c>
+      <c r="C3" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C4" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C5" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>0.001</v>
       </c>
+      <c r="C6" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>0.002</v>
       </c>
+      <c r="C7" s="6" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="C8" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2086,7 +2124,7 @@
         <v>66</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>13</v>
@@ -2130,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>13</v>
@@ -2154,16 +2192,16 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="44.668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="2" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -2175,19 +2213,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -2198,16 +2236,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
@@ -2223,16 +2261,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
@@ -2244,16 +2282,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -2265,16 +2303,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Integrate dynamic stop condition into simulator
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21140" yWindow="460" windowWidth="17040" windowHeight="10700" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23700" windowHeight="11840" tabRatio="989" firstSheet="6" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="148">
   <si>
     <t>Id</t>
   </si>
@@ -492,6 +492,21 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>cond1</t>
+  </si>
+  <si>
+    <t>maxAllowed</t>
+  </si>
+  <si>
+    <t>Test param for testing stop cond1</t>
+  </si>
+  <si>
+    <t>2 &lt; maxAllowed</t>
+  </si>
+  <si>
+    <t>Will always be False</t>
   </si>
 </sst>
 </file>
@@ -502,7 +517,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -535,6 +550,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -572,9 +595,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -619,8 +643,9 @@
     </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1324,15 +1349,22 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1379,6 +1411,20 @@
       </c>
       <c r="G2" s="2" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1390,13 +1436,19 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1404,13 +1456,21 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +2045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>